<commit_message>
Add the Maven Compiler Plugin in pom.xml
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="9420" windowHeight="6615" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="NewUsers" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="NewUsers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -23,62 +23,59 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hobbies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shwetha_54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shwetha998877@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shwetha_511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Playing</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin@email.com</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>Shwetha_511</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Playing</t>
+  </si>
+  <si>
+    <t>Shwetha_56</t>
+  </si>
+  <si>
+    <t>shwetha998879@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,22 +83,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -115,8 +97,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -143,84 +133,48 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -279,62 +233,75 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -387,27 +354,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.85"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -415,7 +381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -425,13 +391,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="admin@email.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="admin@123"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -439,23 +404,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.88"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -478,37 +440,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="shwetha998877@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Deleted unused test cases
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwet\eclipse-workspace\Sush\SeleniumNov2023Batch\SeleniumNovBatch2023\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37C37C2-874A-4BB9-AB97-9FAD5691B036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD99637-7024-449B-9A42-B1509DA59247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,10 +70,10 @@
     <t>Playing</t>
   </si>
   <si>
-    <t>Shwetha_55</t>
-  </si>
-  <si>
-    <t>Shwetha_55@gmail.om</t>
+    <t>Shwetha_56</t>
+  </si>
+  <si>
+    <t>Shwetha_56@gmail.om</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>